<commit_message>
cambios plantilla de cargar estudiantes educativa
</commit_message>
<xml_diff>
--- a/uploads/educativa/plantillaEducativa.xlsx
+++ b/uploads/educativa/plantillaEducativa.xlsx
@@ -30,34 +30,6 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">FE ==&gt; Factura</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="0"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Numero de la factura</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
@@ -71,19 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t xml:space="preserve">NOMBRE_ALUMNO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DOCUMENTO_IDENTIDAD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIPO_DOCUMENTO_PAGO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUM_DOCUMENTO_PAGO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">NOMBRES</t>
   </si>
@@ -105,7 +65,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -130,13 +90,6 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -215,24 +168,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="32.81"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="9" style="0" width="11.5"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32.81"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1018" min="5" style="0" width="11.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1019" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -247,18 +196,6 @@
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios archivo plantilla educativa
</commit_message>
<xml_diff>
--- a/uploads/educativa/plantillaEducativa.xlsx
+++ b/uploads/educativa/plantillaEducativa.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">NOMBRES</t>
   </si>
@@ -55,6 +55,72 @@
   </si>
   <si>
     <t xml:space="preserve">CORREO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dario Granizo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1719534925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GOL201900175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">javierdar5@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alvaro Garcia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0951672849</t>
+  </si>
+  <si>
+    <t xml:space="preserve">201900015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alvarogm2009@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joan Achi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0924131766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joandaniellaachimantilla@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jordan Acaro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0941571069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">201800175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jordanacaro64@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gavriela Aguilar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0925624934</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gabrielaaguilar97@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diana Calderon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0104537980</t>
+  </si>
+  <si>
+    <t xml:space="preserve">201800157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gaby.14x@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -168,10 +234,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -198,6 +264,84 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
cambios en plantilla cargar usuario
</commit_message>
<xml_diff>
--- a/uploads/educativa/plantillaEducativa.xlsx
+++ b/uploads/educativa/plantillaEducativa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC97D8AA-1BD4-419E-8B93-F5EC10EAE097}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4424FE3E-703C-40CF-9A8D-C34C4E8A38DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6639A825-E9D8-4356-89F4-12CAD72E4C30}"/>
   </bookViews>
@@ -95,9 +95,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,28 +417,31 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="6" width="10.90625" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>